<commit_message>
solve lc prob for prac
</commit_message>
<xml_diff>
--- a/LeetCode/Practice.xlsx
+++ b/LeetCode/Practice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Competetive_Programming\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3919C4-B03A-4E0D-9A1D-042D266CDC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04C0C7C-D910-42A9-8DCB-FE3E250FEC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="313">
   <si>
     <t>Status</t>
   </si>
@@ -1416,8 +1416,8 @@
   </sheetPr>
   <dimension ref="A1:I304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1939,7 +1939,9 @@
       <c r="B40" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="C40" s="18"/>
+      <c r="C40" s="18" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="16">
@@ -1957,10 +1959,12 @@
       <c r="A42" s="16">
         <v>38</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="18"/>
+      <c r="C42" s="18" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="16">
@@ -1993,7 +1997,9 @@
       <c r="B45" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="C45" s="18"/>
+      <c r="C45" s="18" t="s">
+        <v>303</v>
+      </c>
       <c r="E45" s="3" t="s">
         <v>6</v>
       </c>
@@ -2008,7 +2014,9 @@
       <c r="B46" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="C46" s="18"/>
+      <c r="C46" s="18" t="s">
+        <v>303</v>
+      </c>
       <c r="F46" s="3" t="s">
         <v>6</v>
       </c>
@@ -2020,7 +2028,9 @@
       <c r="B47" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C47" s="18"/>
+      <c r="C47" s="18" t="s">
+        <v>304</v>
+      </c>
       <c r="E47" s="3" t="s">
         <v>6</v>
       </c>
@@ -2044,7 +2054,9 @@
       <c r="B49" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="C49" s="18"/>
+      <c r="C49" s="18" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="16">
@@ -2053,7 +2065,9 @@
       <c r="B50" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="C50" s="18"/>
+      <c r="C50" s="18" t="s">
+        <v>303</v>
+      </c>
       <c r="E50" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>